<commit_message>
- Fixed some mistakes in BOM.
</commit_message>
<xml_diff>
--- a/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
+++ b/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293E7C6F-85C0-4FCA-BAF9-688FDC1E446E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A130FBC2-501A-4AF2-BA8B-94431B146859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="2325" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="H0FR1" sheetId="1" r:id="rId1"/>
+    <sheet name="H1DR1x-T" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>VLMS1300-GS08</t>
-  </si>
-  <si>
-    <t>VLMO1300-GS08</t>
   </si>
   <si>
     <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp</t>
@@ -299,9 +296,6 @@
     <t>CRCW060310K0JNEB</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
   </si>
   <si>
@@ -311,15 +305,6 @@
     <t>C0603C104K8RACTU</t>
   </si>
   <si>
-    <t xml:space="preserve">AVX </t>
-  </si>
-  <si>
-    <t>0603YC104K4T2A</t>
-  </si>
-  <si>
-    <t>https://octopart.com/0603yc104k4t2a-avx+interconnect+%2F+elco-8120651</t>
-  </si>
-  <si>
     <t>R1, R4, R7</t>
   </si>
   <si>
@@ -329,12 +314,6 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>https://octopart.com/search?q=RC0603FR-07270RL&amp;start=0</t>
-  </si>
-  <si>
-    <t>C3,C5,C6, C10</t>
-  </si>
-  <si>
     <t>LED Uni-Color Soft Yellow 611nm 2-Pin Chip 0603(1608Metric) T/R</t>
   </si>
   <si>
@@ -342,13 +321,37 @@
   </si>
   <si>
     <t>https://octopart.com/vlmy1300-gs08-vishay-21709204?r=sp</t>
+  </si>
+  <si>
+    <t>C3,C5,C6, C10, C12</t>
+  </si>
+  <si>
+    <t>RC0603FR-07270RL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-07270rl-yageo-9288890?r=sp</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>BOURNS_CDSOD323-T03SCBOURNS_CDSOD323-T03SC_0_0</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,13 +423,6 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color theme="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -529,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -580,10 +576,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -592,6 +585,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -612,15 +611,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1000,7 +990,7 @@
   <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1021,7 +1011,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1044,11 +1034,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="23">
         <v>1</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1061,11 +1051,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="24">
         <v>45361</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1073,14 +1063,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
@@ -1116,10 +1106,10 @@
       <c r="D9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1136,16 +1126,16 @@
       <c r="D10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>45</v>
@@ -1156,230 +1146,230 @@
       <c r="D11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="19">
+      <c r="F12" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="56" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>79</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="F13" s="19">
+      <c r="E13" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="19">
+      <c r="E14" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="19">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="18">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="19">
+        <v>73</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="19">
+        <v>57</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="19">
+      <c r="E20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="19">
+        <v>57</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="19">
+      <c r="E22" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1388,20 +1378,20 @@
         <v>33</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
@@ -1414,34 +1404,34 @@
       <c r="D24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>65</v>
-      </c>
       <c r="C25" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="19">
+      <c r="E25" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1454,10 +1444,10 @@
       <c r="D26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="18">
         <v>1</v>
       </c>
     </row>
@@ -1468,27 +1458,26 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E16" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
     <hyperlink ref="E13" r:id="rId6" xr:uid="{3D203CC2-EC47-4D3E-807B-7D07EE67CBE3}"/>
     <hyperlink ref="E14" r:id="rId7" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
-    <hyperlink ref="E17" r:id="rId8" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
+    <hyperlink ref="E16" r:id="rId8" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
     <hyperlink ref="E11" r:id="rId9" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
-    <hyperlink ref="E20" r:id="rId10" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
-    <hyperlink ref="E21" r:id="rId11" xr:uid="{AF654B3F-A2C7-4B2E-B564-D18FD2C0136B}"/>
+    <hyperlink ref="E19" r:id="rId10" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{AF654B3F-A2C7-4B2E-B564-D18FD2C0136B}"/>
     <hyperlink ref="E25" r:id="rId12" xr:uid="{AEA58A7D-7CEF-4AAF-B997-78DCE79302F0}"/>
     <hyperlink ref="E23" r:id="rId13" xr:uid="{5FEE4BAA-3855-4BBB-9484-6712628D4346}"/>
-    <hyperlink ref="E18" r:id="rId14" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
-    <hyperlink ref="E15" r:id="rId15" xr:uid="{2B591E68-3B0C-459F-A99E-A19D9AEB2ADB}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
-    <hyperlink ref="E12" r:id="rId17" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
+    <hyperlink ref="E9" r:id="rId15" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
+    <hyperlink ref="E12" r:id="rId16" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
+    <hyperlink ref="E21" r:id="rId17" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
-  <drawing r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Fixed BOM issues.
</commit_message>
<xml_diff>
--- a/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
+++ b/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A130FBC2-501A-4AF2-BA8B-94431B146859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158DFA47-E3A5-4C24-90D7-5F756C739D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <t>D5</t>
   </si>
   <si>
-    <t>BOURNS_CDSOD323-T03SCBOURNS_CDSOD323-T03SC_0_0</t>
-  </si>
-  <si>
     <t>Bourns</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1210,7 +1210,7 @@
         <v>82</v>
       </c>
       <c r="F14" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -1353,21 +1353,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>97</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="E22" s="22" t="s">
         <v>100</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>101</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
@@ -1389,7 +1389,9 @@
       <c r="E23" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="18"/>
+      <c r="F23" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
@@ -1475,9 +1477,10 @@
     <hyperlink ref="E9" r:id="rId15" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
     <hyperlink ref="E12" r:id="rId16" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
     <hyperlink ref="E21" r:id="rId17" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Everything is finished. I fixed some issues and reviewed everything.
</commit_message>
<xml_diff>
--- a/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
+++ b/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158DFA47-E3A5-4C24-90D7-5F756C739D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A95CFD9-17CB-4E4E-87E3-5F712E1BC9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1DR1x-T" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
   <si>
     <t>Description</t>
   </si>
@@ -154,9 +154,6 @@
     <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
   </si>
   <si>
-    <t>CAP CER 0.1UF 25V X7R 0603</t>
-  </si>
-  <si>
     <t>RES 10K Ohm 1% 0603</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>D3</t>
   </si>
   <si>
@@ -220,24 +214,12 @@
     <t>LED Uni-Color Soft Orange 611nm 2-Pin Chip 0603(1608Metric) T/R</t>
   </si>
   <si>
-    <t>https://octopart.com/vlmo1300-gs08-vishay-21709200?r=sp</t>
-  </si>
-  <si>
     <t xml:space="preserve">RS485 Serial Transceiver (H1DR1x-T) </t>
   </si>
   <si>
     <t>RS-485</t>
   </si>
   <si>
-    <t>Conn Shrouded Header HDR 2 POS 5.08mm Solder ST Thru-Hole</t>
-  </si>
-  <si>
-    <t>https://octopart.com/1546111-2-te+connectivity-40393355</t>
-  </si>
-  <si>
-    <t>AMP 1546111-2</t>
-  </si>
-  <si>
     <t>EAR99 MAX14840 Tape &amp; Reel (TR) RS422RS485 interface driver 3.3V 1.5mA 12ns 40Mbps</t>
   </si>
   <si>
@@ -253,64 +235,12 @@
     <t>C4, C11</t>
   </si>
   <si>
-    <t>https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata </t>
-  </si>
-  <si>
-    <t>GRM21BC81E475KA12L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Murata GRM21BC81E475KA12L
-Multilayer Ceramic Capacitor, GRM Series, 4.7 - F, - 10%, X6S, 25 V, 0805 [2012 Metric</t>
-  </si>
-  <si>
-    <t>R2, R8, R9</t>
-  </si>
-  <si>
     <t>R5</t>
   </si>
   <si>
-    <t>ERJP6WF1200V</t>
-  </si>
-  <si>
-    <t>https://octopart.com/erjp6wf1200v-panasonic-25949195?r=sp#</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Panasonic ERJP6WF1200V
-Res Thick Film 0805 120 Ohm 1% 0.5W(1/2W) ±200ppm/C Pad SMD T/R Automotive AEC-Q200</t>
-  </si>
-  <si>
     <t>R3 , R6</t>
   </si>
   <si>
-    <t>https://octopart.com/crcw060310k0jneb-vishay+dale-46603268</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay </t>
-  </si>
-  <si>
-    <t>CRCW060310K0JNEB</t>
-  </si>
-  <si>
-    <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEMET </t>
-  </si>
-  <si>
-    <t>C0603C104K8RACTU</t>
-  </si>
-  <si>
-    <t>R1, R4, R7</t>
-  </si>
-  <si>
-    <t>270.0R  Thick Film Resistors - SMD 0603</t>
-  </si>
-  <si>
     <t>Yageo</t>
   </si>
   <si>
@@ -326,12 +256,6 @@
     <t>C3,C5,C6, C10, C12</t>
   </si>
   <si>
-    <t>RC0603FR-07270RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0603fr-07270rl-yageo-9288890?r=sp</t>
-  </si>
-  <si>
     <t>D5</t>
   </si>
   <si>
@@ -345,17 +269,92 @@
   </si>
   <si>
     <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>CRCW0603120RFKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/crcw0603120rfkea-vishay-39713744</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>C0805C475K4RACTU</t>
+  </si>
+  <si>
+    <t>KEMET [VA]</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c0805c475k4ractu-kemet-22859922?r=sp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Film Resistors - SMD 0603 270 Ohm 5% Tol	</t>
+  </si>
+  <si>
+    <t>ERJ-3GEYJ271V</t>
+  </si>
+  <si>
+    <t>https://octopart.com/erj-3geyj271v-panasonic-55560546?r=sp</t>
+  </si>
+  <si>
+    <t>TERM BLOCK HEADER (5.08mm) Through Hole 2POS STR Male</t>
+  </si>
+  <si>
+    <t>796636-2</t>
+  </si>
+  <si>
+    <t>https://octopart.com/796636-2-te+connectivity-40130163</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603fr-0710kl-yageo-40025538?r=sp</t>
+  </si>
+  <si>
+    <t>RC0603FR-0710KL</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1 UF 25V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cl10b104ka8nnnc-samsung-19831573?r=sp</t>
+  </si>
+  <si>
+    <t>R2, R4, R7</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>R1, R8, R9</t>
+  </si>
+  <si>
+    <t>VLMO1300-GS08</t>
+  </si>
+  <si>
+    <t>https://octopart.com/vlmo1300-gs08-vishay-21709200</t>
+  </si>
+  <si>
+    <t>23/11/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -363,7 +362,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -374,28 +373,28 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -416,7 +415,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -429,6 +428,13 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -525,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,15 +588,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -611,6 +608,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,9 +647,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2349859</xdr:colOff>
+      <xdr:colOff>2346049</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>16192</xdr:rowOff>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -989,22 +989,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.1796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.19921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="46" x14ac:dyDescent="1">
+    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="6"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
@@ -1015,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1024,7 +1024,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1034,14 +1034,14 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="20">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1051,29 +1051,29 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="24">
-        <v>45361</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
+      <c r="D5" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>34</v>
       </c>
@@ -1106,14 +1106,14 @@
       <c r="D9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="27" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>35</v>
       </c>
@@ -1126,314 +1126,314 @@
       <c r="D10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="27" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="E12" s="27" t="s">
         <v>47</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>96</v>
       </c>
       <c r="F12" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>79</v>
+        <v>55</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>80</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>82</v>
+        <v>16</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="F14" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>85</v>
+        <v>68</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="F15" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E17" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="18">
+      <c r="F17" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="18">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C19" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E19" s="27" t="s">
         <v>25</v>
-      </c>
-      <c r="F18" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>56</v>
       </c>
       <c r="F19" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>93</v>
+        <v>55</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>101</v>
       </c>
       <c r="F21" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>100</v>
+        <v>55</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="F23" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>51</v>
+      <c r="E24" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="F24" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>65</v>
+      <c r="E25" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="F25" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>28</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="D26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F26" s="18">
@@ -1460,27 +1460,24 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E15" r:id="rId5" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{3D203CC2-EC47-4D3E-807B-7D07EE67CBE3}"/>
-    <hyperlink ref="E14" r:id="rId7" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
-    <hyperlink ref="E16" r:id="rId8" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
-    <hyperlink ref="E11" r:id="rId9" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
-    <hyperlink ref="E19" r:id="rId10" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
-    <hyperlink ref="E20" r:id="rId11" xr:uid="{AF654B3F-A2C7-4B2E-B564-D18FD2C0136B}"/>
-    <hyperlink ref="E25" r:id="rId12" xr:uid="{AEA58A7D-7CEF-4AAF-B997-78DCE79302F0}"/>
-    <hyperlink ref="E23" r:id="rId13" xr:uid="{5FEE4BAA-3855-4BBB-9484-6712628D4346}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
-    <hyperlink ref="E9" r:id="rId15" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
-    <hyperlink ref="E12" r:id="rId16" xr:uid="{D2D372F9-DA4F-43C8-B46D-E866F10E6982}"/>
-    <hyperlink ref="E21" r:id="rId17" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
+    <hyperlink ref="E18" r:id="rId1" display="https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ" xr:uid="{D0D8A6B6-6D38-4B73-B861-AACA1609CEF8}"/>
+    <hyperlink ref="E23" r:id="rId2" xr:uid="{F4FAD961-1ACF-40F2-B70C-3F7C4560A218}"/>
+    <hyperlink ref="E22" r:id="rId3" xr:uid="{210F0672-2960-4E6B-9F1A-CB6064DAE39D}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{48762FAB-6BA7-44F3-B66F-9D2208B135F2}"/>
+    <hyperlink ref="E25" r:id="rId5" xr:uid="{5FEE4BAA-3855-4BBB-9484-6712628D4346}"/>
+    <hyperlink ref="E20" r:id="rId6" xr:uid="{301AE570-2045-4255-B607-FD75AE5DA7F8}"/>
+    <hyperlink ref="E12" r:id="rId7" xr:uid="{0A412581-708B-4B43-BCE9-F288010C1F6C}"/>
+    <hyperlink ref="E17" r:id="rId8" xr:uid="{AE63E577-2AF8-4B24-A43D-F4255BA5FD41}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E24" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{7C5636A7-C7CB-4CA9-913E-F76A42FBCF74}"/>
+    <hyperlink ref="E15" r:id="rId14" display="https://octopart.com/crcw060310k0jneb-vishay+dale-46603268" xr:uid="{9CD624AB-68FA-45A0-BDA6-CACF754DD34A}"/>
+    <hyperlink ref="E16" r:id="rId15" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{01DF3B85-9108-476B-8AD5-F1F39BFC2F9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
-  <drawing r:id="rId20"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Fixed description in BOM - Deleted unnecessary file
</commit_message>
<xml_diff>
--- a/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
+++ b/H1DR1x-T/Released/BOM/H1DR1x-T.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\H1DR1x-Hardware\H1DR1x-T\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A95CFD9-17CB-4E4E-87E3-5F712E1BC9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82424C67-4817-419A-9F9D-1B57AEC45BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1DR1x-T" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">TDK </t>
   </si>
   <si>
@@ -344,6 +341,9 @@
   </si>
   <si>
     <t>23/11/2024</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 30 OHM 0603 1LN</t>
   </si>
 </sst>
 </file>
@@ -354,7 +354,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -362,7 +362,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -373,28 +373,28 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -415,7 +415,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -588,6 +588,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -608,9 +611,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -990,21 +990,21 @@
   <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.19921875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" ht="46" x14ac:dyDescent="1">
       <c r="A2" s="6"/>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
@@ -1015,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1024,7 +1024,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1034,46 +1034,46 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="21">
         <v>1</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
+      <c r="D5" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1093,29 +1093,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>37</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>38</v>
+      <c r="E9" s="20" t="s">
+        <v>37</v>
       </c>
       <c r="F9" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>18</v>
@@ -1126,328 +1126,328 @@
       <c r="D10" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="20" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="27" t="s">
-        <v>90</v>
+      <c r="E11" s="20" t="s">
+        <v>89</v>
       </c>
       <c r="F11" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="E12" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>47</v>
       </c>
       <c r="F12" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>80</v>
       </c>
       <c r="F13" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>86</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="27" t="s">
-        <v>87</v>
+      <c r="E14" s="20" t="s">
+        <v>86</v>
       </c>
       <c r="F14" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>91</v>
+      <c r="E15" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="F15" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="D16" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="E16" s="20" t="s">
         <v>95</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>96</v>
       </c>
       <c r="F16" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="20" t="s">
         <v>42</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>43</v>
       </c>
       <c r="F17" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="D18" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="F18" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="E19" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>25</v>
       </c>
       <c r="F19" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="D20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>54</v>
       </c>
       <c r="F20" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>58</v>
-      </c>
       <c r="C21" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>101</v>
       </c>
       <c r="F21" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="D22" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>71</v>
       </c>
       <c r="F22" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="17" t="s">
+      <c r="E23" s="20" t="s">
         <v>75</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="F23" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="E24" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>50</v>
       </c>
       <c r="F24" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>62</v>
       </c>
       <c r="F25" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="28" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="27" t="s">
-        <v>31</v>
+      <c r="E26" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="F26" s="18">
         <v>1</v>

</xml_diff>